<commit_message>
fix excel output, add keyword to birthday
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -489,7 +489,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="1">
-        <v>0</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -509,7 +509,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -537,7 +537,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
@@ -567,7 +567,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <f>SUM(F1:F7)</f>
+        <f>SUM(F1:F9)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>